<commit_message>
Added function to classify post for content pillars
</commit_message>
<xml_diff>
--- a/data/backups/daily_profile_metrics.xlsx
+++ b/data/backups/daily_profile_metrics.xlsx
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -58,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -430,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,10 +530,8 @@
           <t>2025-03-21 15:32:39.461267</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2025-03-21</t>
-        </is>
+      <c r="H2" s="2" t="n">
+        <v>45737</v>
       </c>
       <c r="I2" t="n">
         <v>2025</v>
@@ -584,10 +581,8 @@
           <t>2025-03-22 15:32:56.543004</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2025-03-22</t>
-        </is>
+      <c r="H3" s="2" t="n">
+        <v>45738</v>
       </c>
       <c r="I3" t="n">
         <v>2025</v>
@@ -637,10 +632,8 @@
           <t>2025-03-24 18:24:21.696310</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>2025-03-24</t>
-        </is>
+      <c r="H4" s="2" t="n">
+        <v>45740</v>
       </c>
       <c r="I4" t="n">
         <v>2025</v>
@@ -690,10 +683,8 @@
           <t>2025-03-27 20:18:11.265210</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2025-03-27</t>
-        </is>
+      <c r="H5" s="2" t="n">
+        <v>45743</v>
       </c>
       <c r="I5" t="n">
         <v>2025</v>
@@ -743,10 +734,8 @@
           <t>2025-03-29 23:20:39.406798</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>2025-03-29</t>
-        </is>
+      <c r="H6" s="2" t="n">
+        <v>45745</v>
       </c>
       <c r="I6" t="n">
         <v>2025</v>
@@ -796,10 +785,8 @@
           <t>2025-03-30 23:20:48.817247</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>2025-03-30</t>
-        </is>
+      <c r="H7" s="2" t="n">
+        <v>45746</v>
       </c>
       <c r="I7" t="n">
         <v>2025</v>
@@ -849,10 +836,8 @@
           <t>2025-03-31 23:21:04.347441</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>2025-03-31</t>
-        </is>
+      <c r="H8" s="2" t="n">
+        <v>45747</v>
       </c>
       <c r="I8" t="n">
         <v>2025</v>
@@ -902,10 +887,8 @@
           <t>2025-04-01 16:52:19.058239</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>2025-04-01</t>
-        </is>
+      <c r="H9" s="2" t="n">
+        <v>45748</v>
       </c>
       <c r="I9" t="n">
         <v>2025</v>
@@ -955,10 +938,8 @@
           <t>2025-04-02 16:52:40.013681</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>2025-04-02</t>
-        </is>
+      <c r="H10" s="2" t="n">
+        <v>45749</v>
       </c>
       <c r="I10" t="n">
         <v>2025</v>
@@ -1008,10 +989,8 @@
           <t>2025-04-03 16:53:01.376215</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>2025-04-03</t>
-        </is>
+      <c r="H11" s="2" t="n">
+        <v>45750</v>
       </c>
       <c r="I11" t="n">
         <v>2025</v>
@@ -1061,10 +1040,8 @@
           <t>2025-04-04 16:52:22.718804</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>2025-04-04</t>
-        </is>
+      <c r="H12" s="2" t="n">
+        <v>45751</v>
       </c>
       <c r="I12" t="n">
         <v>2025</v>
@@ -1114,10 +1091,8 @@
           <t>2025-04-07 00:50:29.998578</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>2025-04-07</t>
-        </is>
+      <c r="H13" s="2" t="n">
+        <v>45754</v>
       </c>
       <c r="I13" t="n">
         <v>2025</v>
@@ -1167,10 +1142,8 @@
           <t>2025-04-08 20:03:49.900666</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>2025-04-08</t>
-        </is>
+      <c r="H14" s="2" t="n">
+        <v>45755</v>
       </c>
       <c r="I14" t="n">
         <v>2025</v>
@@ -1220,10 +1193,8 @@
           <t>2025-04-11 11:03:02.012559</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>2025-04-11</t>
-        </is>
+      <c r="H15" s="2" t="n">
+        <v>45758</v>
       </c>
       <c r="I15" t="n">
         <v>2025</v>
@@ -1273,10 +1244,8 @@
           <t>2025-04-12 11:02:50.473294</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>2025-04-12</t>
-        </is>
+      <c r="H16" s="2" t="n">
+        <v>45759</v>
       </c>
       <c r="I16" t="n">
         <v>2025</v>
@@ -1326,10 +1295,8 @@
           <t>2025-04-13 11:02:18.007481</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>2025-04-13</t>
-        </is>
+      <c r="H17" s="2" t="n">
+        <v>45760</v>
       </c>
       <c r="I17" t="n">
         <v>2025</v>
@@ -1379,10 +1346,8 @@
           <t>2025-04-14 11:02:45.751306</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>2025-04-14</t>
-        </is>
+      <c r="H18" s="2" t="n">
+        <v>45761</v>
       </c>
       <c r="I18" t="n">
         <v>2025</v>
@@ -1424,18 +1389,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=RYd0qaB1w1UQ7kNvwGTSFBA&amp;_nc_oc=AdnFH6UuR7J54h90SPGdIiHD7R7sFdakB_5MyW6UFe4fBoFDLtdKr8ZWr9AurwK3dEVsZCVk2-jVr_1Ftdmfo9yN&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHpj314dbbaNyIQKL6fYUAKrdhVV-HuaB_4cmNL7t8fZw&amp;oe=680471AE</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G19" s="3" t="n">
-        <v>45762.45992217593</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>2025-04-15</t>
-        </is>
+      <c r="F19" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>2025-04-15 11:02:17.275604</t>
+        </is>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>45762</v>
       </c>
       <c r="I19" t="n">
         <v>2025</v>
@@ -1477,18 +1440,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=RYd0qaB1w1UQ7kNvwFOJALO&amp;_nc_oc=AdmaCb-kgpNBdV82RqeJaYpZSuEPerXSAbiFALQdu1rf72F_lD-1dsLSMs_-ppn1d_OFboDGOTns21OR632dPk9U&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfGfG12WGh8zf39_kw4xAslqvJVP9Hif_8l_4EF97U2Gbg&amp;oe=6805C32E</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="n">
-        <v>45763.46002614583</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>2025-04-16</t>
-        </is>
+      <c r="F20" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>2025-04-16 11:02:26.258788</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>45763</v>
       </c>
       <c r="I20" t="n">
         <v>2025</v>
@@ -1530,18 +1491,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Q1PwlYQfxIAQ7kNvwE-0L8h&amp;_nc_oc=Adlsikp9RAiod7K9kuuUWb66l5vykEvAtLTz0G8T1ZFlDIkJCFU9RxH9JCcEwWcfp-SPnVQz3fCu0qo9dviByoJ_&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHfmeGXr2QJcc2915QtPT8RMYIKc7xoqs-qVcgHTjl2NA&amp;oe=680714AE</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G21" s="3" t="n">
-        <v>45764.46059219907</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>2025-04-17</t>
-        </is>
+      <c r="F21" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>2025-04-17 11:03:15.165666</t>
+        </is>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>45764</v>
       </c>
       <c r="I21" t="n">
         <v>2025</v>
@@ -1583,18 +1542,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Q1PwlYQfxIAQ7kNvwGcuOtg&amp;_nc_oc=AdncBWRow9UEvlpW9sJA0x86gmLawVhipChPPQSlcnYO4CdEDQv7_j1ReGa_nRP78y9ndmO1_3scTIiTIizfAGdh&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfFJDU3uh-NZMDPVEUgCXGP0HAT7DFAb8dJoChXdlo9jJQ&amp;oe=6808662E</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G22" s="3" t="n">
-        <v>45765.46053376157</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>2025-04-18</t>
-        </is>
+      <c r="F22" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>2025-04-18 11:03:10.117092</t>
+        </is>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>45765</v>
       </c>
       <c r="I22" t="n">
         <v>2025</v>
@@ -1636,18 +1593,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Q1PwlYQfxIAQ7kNvwHOB_yW&amp;_nc_oc=Adk1ZQ2ci8oHu8p-80tyIPRtoST1pxpoHBG7yOJKonpHbwsbOf9Qff39HFpfnKHU6AbpEzuQe1Xw83AvMtSin9N4&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfEvP4vm3NfQVz2wQ0ns6ufeqeM3Uviekrb6eP__KNlmiw&amp;oe=6809B7AE</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G23" s="3" t="n">
-        <v>45766.4603133912</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>2025-04-19</t>
-        </is>
+      <c r="F23" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>2025-04-19 11:02:51.076562</t>
+        </is>
+      </c>
+      <c r="H23" s="2" t="n">
+        <v>45766</v>
       </c>
       <c r="I23" t="n">
         <v>2025</v>
@@ -1689,18 +1644,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=eqWF18t31ggQ7kNvwHNTkkM&amp;_nc_oc=AdnuPd9vVOReKHEv_Vq9gKjrOxi8DEA_7Ahlfp1Hm50Np8tPMqdVrEPDWAOXX8UjKUz3nE9dl6znJQl5Wv9hyjAj&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHrAlHlMkx09NREs3CUNeQ2CBMgOWIJUbguXeXiqwCrQA&amp;oe=680CCB2E</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G24" s="3" t="n">
-        <v>45768.7933908912</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>2025-04-21</t>
-        </is>
+      <c r="F24" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>2025-04-21 19:02:28.973359</t>
+        </is>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>45768</v>
       </c>
       <c r="I24" t="n">
         <v>2025</v>
@@ -1742,18 +1695,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5i3I2csq8uEQ7kNvwEKz7Yd&amp;_nc_oc=AdkRxlM2NhmFwZChQ-1RnUDWaqX_vAAmCy-fhfu94Z5keiJh8_SfO4e89iiSPWAqwel-RsdAh1j_aeVvDQsKaJes&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfE7x0LSIsOvY-TiGQvBzNIP9D0Fe2zUoADhrQ1yAnFEBA&amp;oe=680F6E2E</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G25" s="3" t="n">
-        <v>45770.7963471875</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>2025-04-23</t>
-        </is>
+      <c r="F25" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>2025-04-23 19:06:44.396996</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>45770</v>
       </c>
       <c r="I25" t="n">
         <v>2025</v>
@@ -1795,18 +1746,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5i3I2csq8uEQ7kNvwEKz7Yd&amp;_nc_oc=AdkRxlM2NhmFwZChQ-1RnUDWaqX_vAAmCy-fhfu94Z5keiJh8_SfO4e89iiSPWAqwel-RsdAh1j_aeVvDQsKaJes&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHG4diHIh7SU3gjVOu5fkdMttfXSGTzU9jTO2qqkGORfQ&amp;oe=6810BFAE</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G26" s="3" t="n">
-        <v>45771.79633731482</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>2025-04-24</t>
-        </is>
+      <c r="F26" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2025-04-24 19:06:43.543960</t>
+        </is>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>45771</v>
       </c>
       <c r="I26" t="n">
         <v>2025</v>
@@ -1848,18 +1797,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5i3I2csq8uEQ7kNvwEd9nit&amp;_nc_oc=AdmNe1DW6nxiUXbe-r79DYo9FCi9MstBagIYW2455H7uXgc3fWF342dH6SMHA8ThixfnA11WE6tXNUo4fVjSGF4i&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfFHDDBhGBMR81TiGCam1ftLilQWf2V6jlpzyBDxdSfN1g&amp;oe=6812112E</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G27" s="3" t="n">
-        <v>45772.79676655093</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>2025-04-25</t>
-        </is>
+      <c r="F27" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>2025-04-25 19:07:20.629981</t>
+        </is>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>45772</v>
       </c>
       <c r="I27" t="n">
         <v>2025</v>
@@ -1901,18 +1848,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Dz02SseckA4Q7kNvwGK4onp&amp;_nc_oc=Adk5bZBxkx5XVNu2nW5PFK9tL6pDx60g7xbNxR-LkfgGj-bRn6XaFOV-9J8LvIHtNVQpylakm6uLBfhKtqWkbh6T&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfG4-d4a6YXunqUtl0kbO8hAEBlGMgzn1srlgQR7iYg4SQ&amp;oe=681362AE</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G28" s="3" t="n">
-        <v>45773.79669516204</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>2025-04-26</t>
-        </is>
+      <c r="F28" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-04-26 19:07:14.462028</t>
+        </is>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>45773</v>
       </c>
       <c r="I28" t="n">
         <v>2025</v>
@@ -1954,18 +1899,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Dz02SseckA4Q7kNvwF0SWeh&amp;_nc_oc=AdloBVgDfoo_05jlgC74GtM3-OlzHeHmau2AATCGilmtDiR0Vx7wyBGFnhCZsEPl6vT3iQi80dj14jFpnmwo-Uhm&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHDod5xns9gCB4HbPHARzqU95NU17n4wkCbjgrFa0wW4w&amp;oe=6814B42E</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G29" s="3" t="n">
-        <v>45774.79626265046</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>2025-04-27</t>
-        </is>
+      <c r="F29" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-04-27 19:06:37.093066</t>
+        </is>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>45774</v>
       </c>
       <c r="I29" t="n">
         <v>2025</v>
@@ -2007,18 +1950,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=Dz02SseckA4Q7kNvwFVwDiC&amp;_nc_oc=AdkljOA40prPAIhkPVdr6XHgt5nNh13X9uCtyJevaoM8sjoGTnqS1XHiz10YziJOjRmdiOFKlsSR9kfSg4oRXYxn&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfH0CDz3OUKpX4Ut3hBYfZ23g9cQ5ngmClSw6XtYxeSp7w&amp;oe=681605AE</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G30" s="3" t="n">
-        <v>45775.79613978009</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>2025-04-28</t>
-        </is>
+      <c r="F30" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-04-28 19:06:26.476910</t>
+        </is>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>45775</v>
       </c>
       <c r="I30" t="n">
         <v>2025</v>
@@ -2060,18 +2001,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=28p1nT6RoOEQ7kNvwG07osv&amp;_nc_oc=AdmOq0dMbzeCVTYkuwGrkKSM7SM6tCqKy8i_i1wNVqWW8TBy2220Wv1ZEyTOvVVe5IAEXdc0NpPUroGJE3eoXrjo&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfGjlaztThhmMaimy2eW9XO81914jAhWEskkcaXzx37jXg&amp;oe=6817572E</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G31" s="3" t="n">
-        <v>45776.79649628473</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>2025-04-29</t>
-        </is>
+      <c r="F31" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2025-04-29 19:06:57.278762</t>
+        </is>
+      </c>
+      <c r="H31" s="2" t="n">
+        <v>45776</v>
       </c>
       <c r="I31" t="n">
         <v>2025</v>
@@ -2113,18 +2052,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=28p1nT6RoOEQ7kNvwHGZR9P&amp;_nc_oc=AdnwGTSlb6ySVsLjYhJjInyCp2uQZMk7vJ8qwV6r9_HwXNDuo115nPFuHDebqQSeS2WpnWOSoDhb9RBag8G0gX8S&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfFcwSZRbyRhg4LNNX6NYeTxO08mlcc3I0PpV6NSiCcCvA&amp;oe=6818A8AE</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G32" s="3" t="n">
-        <v>45777.79628887732</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>2025-04-30</t>
-        </is>
+      <c r="F32" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-04-30 19:06:39.359292</t>
+        </is>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>45777</v>
       </c>
       <c r="I32" t="n">
         <v>2025</v>
@@ -2166,18 +2103,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=IN_GzJ2sEioQ7kNvwEg5sAD&amp;_nc_oc=AdmbXpAWtsQMCdIwbFTEUc4JIrzUeJ9uIJ4C1O82AyJcxE37ZsWHolsvcoPOTNlvUekXXV9pY0xppZrwjtvdwQuG&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfF2KCp5eD5JwgsRqqE5k-h6S6kr-WVqzqPMiZpcYcAfiA&amp;oe=681AA2EE</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G33" s="3" t="n">
-        <v>45779.39787231482</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>2025-05-02</t>
-        </is>
+      <c r="F33" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-05-02 09:32:56.167637</t>
+        </is>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>45779</v>
       </c>
       <c r="I33" t="n">
         <v>2025</v>
@@ -2219,18 +2154,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=IN_GzJ2sEioQ7kNvwEqMVvT&amp;_nc_oc=Adn9AyAP7zVKP8mCM-NlEfWXWDn0EUPNIDmmlWymEbMxy_VQTH1j2nzPajVTTI-IyX7LCUt3-J_BFTygH72RmzK3&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHdpU4Tt9hgkmkwxmNbcV03t3tVxjWexSSwb3ifD4AmOQ&amp;oe=681BF46E</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G34" s="3" t="n">
-        <v>45780.39800649306</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>2025-05-03</t>
-        </is>
+      <c r="F34" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-05-03 09:33:07.761292</t>
+        </is>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>45780</v>
       </c>
       <c r="I34" t="n">
         <v>2025</v>
@@ -2272,18 +2205,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=IN_GzJ2sEioQ7kNvwEg5sAD&amp;_nc_oc=AdmbXpAWtsQMCdIwbFTEUc4JIrzUeJ9uIJ4C1O82AyJcxE37ZsWHolsvcoPOTNlvUekXXV9pY0xppZrwjtvdwQuG&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfFQOke_4Tg7xiVQUNcuQXo67qvYOZgww0dl-EkFtkq7Ww&amp;oe=681D45EE</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G35" s="3" t="n">
-        <v>45781.39785303241</v>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>2025-05-04</t>
-        </is>
+      <c r="F35" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-05-04 09:32:54.502485</t>
+        </is>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>45781</v>
       </c>
       <c r="I35" t="n">
         <v>2025</v>
@@ -2325,18 +2256,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=NWtNeasGJ7MQ7kNvwFv6SEU&amp;_nc_oc=Adl4mAinciDaL3ehOoV15zVu7rknF2pd7VX55SvNk7sVYaKBpUDwGi7Jq52lF0FmLp7QfmpP3mLsnvLUT7T1A-Sm&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfHcbyEFnu0D8TK_-SHc-MnU6EbB3y2P69duW_FBMW99bA&amp;oe=681E976E</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G36" s="3" t="n">
-        <v>45782.40760672454</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>2025-05-05</t>
-        </is>
+      <c r="F36" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-05-05 09:46:57.220598</t>
+        </is>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>45782</v>
       </c>
       <c r="I36" t="n">
         <v>2025</v>
@@ -2378,18 +2307,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=NWtNeasGJ7MQ7kNvwFv6SEU&amp;_nc_oc=Adl4mAinciDaL3ehOoV15zVu7rknF2pd7VX55SvNk7sVYaKBpUDwGi7Jq52lF0FmLp7QfmpP3mLsnvLUT7T1A-Sm&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfKR6iib3jExJe38KR9WHOoXEmZ7y1ZaJmiaEMtZ4Q4gYQ&amp;oe=681FE8EE</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G37" s="3" t="n">
-        <v>45783.39771293981</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>2025-05-06</t>
-        </is>
+      <c r="F37" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-05-06 09:32:42.397749</t>
+        </is>
+      </c>
+      <c r="H37" s="2" t="n">
+        <v>45783</v>
       </c>
       <c r="I37" t="n">
         <v>2025</v>
@@ -2431,18 +2358,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=NWtNeasGJ7MQ7kNvwFv6SEU&amp;_nc_oc=Adl4mAinciDaL3ehOoV15zVu7rknF2pd7VX55SvNk7sVYaKBpUDwGi7Jq52lF0FmLp7QfmpP3mLsnvLUT7T1A-Sm&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfKhIWqa2E3vK2KuY1WvA1T7IkZMBZDSDA2J_HgJZp_hXw&amp;oe=68213A6E</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G38" s="3" t="n">
-        <v>45784.39764586806</v>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>2025-05-07</t>
-        </is>
+      <c r="F38" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-05-07 09:32:36.602758</t>
+        </is>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>45784</v>
       </c>
       <c r="I38" t="n">
         <v>2025</v>
@@ -2484,18 +2409,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=0AU5y29RBJMQ7kNvwG0fiXo&amp;_nc_oc=Adm6mtt-VWMmU47z_8dZcs8ZohztvDlKlvxT8c_mrNeBEpKue1MFDM6mNXCVGzOu5cmSkClZFSB2bAzP98sevVfi&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfJhxJX46NBaVXEX2MrzjBlSB1VdmWaCba61JaW8dMi86A&amp;oe=68228BEE</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G39" s="3" t="n">
-        <v>45785.39818737269</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>2025-05-08</t>
-        </is>
+      <c r="F39" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-05-08 09:33:23.389117</t>
+        </is>
+      </c>
+      <c r="H39" s="2" t="n">
+        <v>45785</v>
       </c>
       <c r="I39" t="n">
         <v>2025</v>
@@ -2537,18 +2460,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=0AU5y29RBJMQ7kNvwFl-fOI&amp;_nc_oc=AdmC-OprH3Cbhp3s-2CBBrKKIWxNfyNh-7gYSoCwds5tNlOSVtv23jaLv7QJoH9Oqp-fKP8TUYosaQdDqdrVHnqj&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfJWCt6ApHgyf78T5VAwlD277JTJgC_WJVb--fiocoFkxA&amp;oe=6823DD6E</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G40" s="3" t="n">
-        <v>45786.39813979167</v>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>2025-05-09</t>
-        </is>
+      <c r="F40" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-05-09 09:33:19.277721</t>
+        </is>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>45786</v>
       </c>
       <c r="I40" t="n">
         <v>2025</v>
@@ -2590,18 +2511,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=0AU5y29RBJMQ7kNvwFpX11s&amp;_nc_oc=AdlpXoSD_0bybCq1WNU1em450t9VxY0rAF519qzRUMnNfHN8bjVZtp-epfLj91LZ1Ub5tE3yQZi2vUG5XqwD9MCS&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfIRWnTm4YydRQ4X3NssjvKZfbW9KFgSkGxIxdremZ9JZg&amp;oe=68252EEE</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G41" s="3" t="n">
-        <v>45787.39810366898</v>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>2025-05-10</t>
-        </is>
+      <c r="F41" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-05-10 09:33:16.156526</t>
+        </is>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>45787</v>
       </c>
       <c r="I41" t="n">
         <v>2025</v>
@@ -2643,18 +2562,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=98Z30Y-Fn84Q7kNvwGigcY3&amp;_nc_oc=AdnlmqP0Owtm9g4fPHIQtb0Rs-3ny1ApT5-BOO0J8fyh8uZsEbvN01ZdKBP2dzXKBWBYiGD6BG8VmcDe86MNKr2X&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfI74XBNz4sZmfpTCCRLRUo6v8FSnNHdPQSIPqEIpumutQ&amp;oe=6826806E</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G42" s="3" t="n">
-        <v>45788.39804859953</v>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>2025-05-11</t>
-        </is>
+      <c r="F42" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-05-11 09:33:11.398732</t>
+        </is>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>45788</v>
       </c>
       <c r="I42" t="n">
         <v>2025</v>
@@ -2696,18 +2613,16 @@
           <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=98Z30Y-Fn84Q7kNvwFG_Vub&amp;_nc_oc=AdlBhQs5yoAx2HX9ehwQEDxKusa4_dxclDLJsZm2zFF7LvHd2ATdglLLxKuRHjvPxDybk4J6fG9sXmCu5a9P_MPF&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfIFkVgVIEsFPA10mlaTSX0D9GLV76yK-VCA3k6ArQ6NAw&amp;oe=6827D1EE</t>
         </is>
       </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>17841461458191255</t>
-        </is>
-      </c>
-      <c r="G43" s="3" t="n">
-        <v>45789.42137029266</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>2025-05-12</t>
-        </is>
+      <c r="F43" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-05-12 10:06:46.393286</t>
+        </is>
+      </c>
+      <c r="H43" s="2" t="n">
+        <v>45789</v>
       </c>
       <c r="I43" t="n">
         <v>2025</v>
@@ -2723,6 +2638,2002 @@
       <c r="L43" t="inlineStr">
         <is>
           <t>10:06:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>2984</v>
+      </c>
+      <c r="C44" t="n">
+        <v>238</v>
+      </c>
+      <c r="D44" t="n">
+        <v>174</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=98Z30Y-Fn84Q7kNvwFG_Vub&amp;_nc_oc=AdlBhQs5yoAx2HX9ehwQEDxKusa4_dxclDLJsZm2zFF7LvHd2ATdglLLxKuRHjvPxDybk4J6fG9sXmCu5a9P_MPF&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfJ-Y6F611Y1W1BQhsDBLCP4JvvrgYAWu8LlVQrb2jg1fw&amp;oe=68295BAE</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-05-13 14:15:28.403731</t>
+        </is>
+      </c>
+      <c r="H44" s="2" t="n">
+        <v>45790</v>
+      </c>
+      <c r="I44" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K44" t="n">
+        <v>13</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>14:15:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>2982</v>
+      </c>
+      <c r="C45" t="n">
+        <v>239</v>
+      </c>
+      <c r="D45" t="n">
+        <v>175</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=AFwoBlpIDm4Q7kNvwE9fGju&amp;_nc_oc=AdlngE2KRzEw2y0Q4bGJdvPJinlvT2O2mDt7_-2RSxZKlVlMZFA9SRlApZroZsGvMCkYFv6NtRbi7ZXAQ3rUPYvU&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfKVjGFQjdzYa3u-r0OWU7OyfZyBxt2Kw2ssC04wvjPgMA&amp;oe=682B1DAE</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-05-14 19:07:45.984611</t>
+        </is>
+      </c>
+      <c r="H45" s="2" t="n">
+        <v>45791</v>
+      </c>
+      <c r="I45" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>14</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>19:07:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>2983</v>
+      </c>
+      <c r="C46" t="n">
+        <v>239</v>
+      </c>
+      <c r="D46" t="n">
+        <v>178</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=AFwoBlpIDm4Q7kNvwE9fGju&amp;_nc_oc=AdlngE2KRzEw2y0Q4bGJdvPJinlvT2O2mDt7_-2RSxZKlVlMZFA9SRlApZroZsGvMCkYFv6NtRbi7ZXAQ3rUPYvU&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfJKHOWm4myvXJzuX8ytjhnpossedHlTAcDvttghIur4kg&amp;oe=682C6F2E</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-05-15 19:07:38.181039</t>
+        </is>
+      </c>
+      <c r="H46" s="2" t="n">
+        <v>45792</v>
+      </c>
+      <c r="I46" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K46" t="n">
+        <v>15</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>19:07:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>2987</v>
+      </c>
+      <c r="C47" t="n">
+        <v>239</v>
+      </c>
+      <c r="D47" t="n">
+        <v>179</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=AFwoBlpIDm4Q7kNvwE9fGju&amp;_nc_oc=AdlngE2KRzEw2y0Q4bGJdvPJinlvT2O2mDt7_-2RSxZKlVlMZFA9SRlApZroZsGvMCkYFv6NtRbi7ZXAQ3rUPYvU&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfI5QtHXdsWTqDdO2_7XzSveRN12akNRSjX3j-Lfd3Lk8Q&amp;oe=682DC0AE</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-05-16 19:07:34.166399</t>
+        </is>
+      </c>
+      <c r="H47" s="2" t="n">
+        <v>45793</v>
+      </c>
+      <c r="I47" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K47" t="n">
+        <v>16</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>19:07:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>2991</v>
+      </c>
+      <c r="C48" t="n">
+        <v>239</v>
+      </c>
+      <c r="D48" t="n">
+        <v>179</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=CTYyAecaZqwQ7kNvwHALtmS&amp;_nc_oc=AdlPmix6ZotxHoAn7oIMgFXCgX4erC4VGI_ZBRt2yeLySn09NJLz_LZbEniKCn2snDNV45R_KvhpPhG66dDTd-hH&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfL95JGydpEQEzkmKNbHllNOHU082K1JSJNQVUtjIcLvBg&amp;oe=682F122E</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-05-17 19:08:17.541935</t>
+        </is>
+      </c>
+      <c r="H48" s="2" t="n">
+        <v>45794</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>17</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>19:08:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>2994</v>
+      </c>
+      <c r="C49" t="n">
+        <v>239</v>
+      </c>
+      <c r="D49" t="n">
+        <v>179</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=CTYyAecaZqwQ7kNvwHS4RyP&amp;_nc_oc=Adk8WyFDh06mEZUAog_u9eoXnSl448_D_iRSxrLr3a3ZUb_vpjDUvuF93sfraXfmhqGkwndDV74OIpIgF7FyXMvp&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfImmD7hqOhtWkrra2ox7MauquZ0NQf6qDId_jqmsPDqjQ&amp;oe=683063AE</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-05-18 19:07:33.116947</t>
+        </is>
+      </c>
+      <c r="H49" s="2" t="n">
+        <v>45795</v>
+      </c>
+      <c r="I49" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
+        <v>18</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>19:07:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>2991</v>
+      </c>
+      <c r="C50" t="n">
+        <v>237</v>
+      </c>
+      <c r="D50" t="n">
+        <v>180</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=CTYyAecaZqwQ7kNvwHt4H9a&amp;_nc_oc=AdkAK1nCJN5NR8LxqGpHygyWVXnZ3rPGyjoZlDtg6bDYjB4EOcvFVxFt5dLNIlxIZYsvs1-7psUd1N32qdLbIoKD&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfLDK5wrPO6Y3jjGiI36C3TD-mg5vhfm1XYO1cEcEAMoCw&amp;oe=6831B52E</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-05-19 19:08:22.180489</t>
+        </is>
+      </c>
+      <c r="H50" s="2" t="n">
+        <v>45796</v>
+      </c>
+      <c r="I50" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>19</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>19:08:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>2996</v>
+      </c>
+      <c r="C51" t="n">
+        <v>237</v>
+      </c>
+      <c r="D51" t="n">
+        <v>182</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=6fJVGczCPXYQ7kNvwF00Hbg&amp;_nc_oc=Adlxvu0cAgWXnV7RtExcrg5vY8Jwb8Wa7oVbUkoC80UAr3Rz9jgbgSuDmGqIdxI_qG_zKvdr8ISxj8u5vkv5sis9&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfIeqhZU_BDBpWP8hwMhf9HmSi3pC3CvHT5JSuMO1nX3Cw&amp;oe=683306AE</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-05-20 19:07:54.143686</t>
+        </is>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>45797</v>
+      </c>
+      <c r="I51" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>20</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>19:07:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>3001</v>
+      </c>
+      <c r="C52" t="n">
+        <v>238</v>
+      </c>
+      <c r="D52" t="n">
+        <v>183</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=6fJVGczCPXYQ7kNvwFDY0mx&amp;_nc_oc=Adlv0703leE61OoAE7AQ8rvnALa-ZUtg1KxlcS0bj_mO3ovTS_xEol722rhXIj2qtKQEe8sl22dZhrc6DTeUhvUS&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfJbPvJasx5oUoeMu_IXkxNhTnZ6MqxW2nIFgM8a7GxmfQ&amp;oe=6834582E</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2025-05-21 19:07:57.763826</t>
+        </is>
+      </c>
+      <c r="H52" s="2" t="n">
+        <v>45798</v>
+      </c>
+      <c r="I52" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K52" t="n">
+        <v>21</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>19:07:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>3008</v>
+      </c>
+      <c r="C53" t="n">
+        <v>238</v>
+      </c>
+      <c r="D53" t="n">
+        <v>184</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=6fJVGczCPXYQ7kNvwEab-53&amp;_nc_oc=AdlSHfEmIy-RmTmOh0mE5Cc13P2Csr-QxXBKN1i9c0E33l6q7xZjqRYmfNSZx0XQgOdVuJgsoixz-t1kxVAe-1SD&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfIZiboOdQ5wiKHrb_1fCsiBK6-HW3PPe7dDCI_rXPzEkQ&amp;oe=6835A9AE</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2025-05-22 19:08:01.082221</t>
+        </is>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>45799</v>
+      </c>
+      <c r="I53" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K53" t="n">
+        <v>22</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>19:08:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>3006</v>
+      </c>
+      <c r="C54" t="n">
+        <v>239</v>
+      </c>
+      <c r="D54" t="n">
+        <v>185</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=LNkvZyc6d9gQ7kNvwF8Kvlg&amp;_nc_oc=AdmeYqDOtgP0Y06yVGRVhJLkSbcTCk1gmKjPEuKDBJ0PRHktszIUCu6DzrqPixR7PNtBaWWXxZwywW-wre3FBHAL&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfIUs4oQ8fUTGOjbhe9Yrj1n8U2eL-FZh0LEYrM5wvbVwQ&amp;oe=6836FB2E</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2025-05-23 19:08:26.283591</t>
+        </is>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>45800</v>
+      </c>
+      <c r="I54" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K54" t="n">
+        <v>23</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>19:08:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>3030</v>
+      </c>
+      <c r="C55" t="n">
+        <v>242</v>
+      </c>
+      <c r="D55" t="n">
+        <v>187</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=FzDDKfhxSSEQ7kNvwFJ-Bg1&amp;_nc_oc=AdnRm4u2kWENq7Ub6-ggqM6cOeam2i_H7-QrwOg2VzGBnY6zM5c3POqT_vbOzXpYHaTsErXRSlwt6rnq9t23TU3F&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfLbXpfWdJ1Hz5RYNOZBsBavHoU-f5e2AGwI1BDlu0ApXw&amp;oe=683AEFAE</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2025-05-26 22:32:16.922442</t>
+        </is>
+      </c>
+      <c r="H55" s="2" t="n">
+        <v>45803</v>
+      </c>
+      <c r="I55" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K55" t="n">
+        <v>26</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>22:32:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>3043</v>
+      </c>
+      <c r="C56" t="n">
+        <v>242</v>
+      </c>
+      <c r="D56" t="n">
+        <v>188</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=FzDDKfhxSSEQ7kNvwGNDNIf&amp;_nc_oc=Adnl9CyWDo2rw2ohWz98DrTQZoyUUCLpsb36l5tkGsAHfexaijITdSXcTef2osGl4YOeL5czgwWkyQfGbetXD45d&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfJEb7CJgXE3nDOeAolVdKKMeqPfvM8tKWjdbEfV5IzDRg&amp;oe=683C412E</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2025-05-27 22:32:02.711972</t>
+        </is>
+      </c>
+      <c r="H56" s="2" t="n">
+        <v>45804</v>
+      </c>
+      <c r="I56" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K56" t="n">
+        <v>27</v>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>22:32:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>3049</v>
+      </c>
+      <c r="C57" t="n">
+        <v>242</v>
+      </c>
+      <c r="D57" t="n">
+        <v>189</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=FzDDKfhxSSEQ7kNvwGNDNIf&amp;_nc_oc=Adnl9CyWDo2rw2ohWz98DrTQZoyUUCLpsb36l5tkGsAHfexaijITdSXcTef2osGl4YOeL5czgwWkyQfGbetXD45d&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfKBxdBQryq0F6kJBQy8TLg_9oCcPKGm1JjXzsdpNHkG2w&amp;oe=683D92AE</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2025-05-28 22:32:23.270995</t>
+        </is>
+      </c>
+      <c r="H57" s="2" t="n">
+        <v>45805</v>
+      </c>
+      <c r="I57" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="K57" t="n">
+        <v>28</v>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>22:32:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>3070</v>
+      </c>
+      <c r="C58" t="n">
+        <v>243</v>
+      </c>
+      <c r="D58" t="n">
+        <v>192</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=fIEW47mq72EQ7kNvwGKsPwf&amp;_nc_oc=AdmdnLkywwMXSG8xU8gTvFo2tjPqFjjcwpmUg8kM4fnwQUmJWn_92JgZz6HY0QN_ThYsJVvWBSfGUlqm1qb3w2Ka&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfJLylwqV_KeTLP--m-GQ_NXzhkdAlgmKAjDjVKNb6658w&amp;oe=6842D8AE</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2025-06-01 19:07:25.647213</t>
+        </is>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>45809</v>
+      </c>
+      <c r="I58" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K58" t="n">
+        <v>1</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>19:07:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>3077</v>
+      </c>
+      <c r="C59" t="n">
+        <v>243</v>
+      </c>
+      <c r="D59" t="n">
+        <v>192</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=fIEW47mq72EQ7kNvwGV_iLz&amp;_nc_oc=AdkGma694nv-suwH26OS-Ho-plpF4GNy6j0v6XR2WLM7uTudtbHAzkrfQIhEdScHIWTuF7EX0sdZruXCFRQV0IBA&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfL8Nz60En56_Lv5OhKLCG8jtIFhQFYq-lzaJkIvj34fGA&amp;oe=68442A2E</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2025-06-02 19:37:53.766435</t>
+        </is>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>45810</v>
+      </c>
+      <c r="I59" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K59" t="n">
+        <v>2</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>19:37:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>3079</v>
+      </c>
+      <c r="C60" t="n">
+        <v>246</v>
+      </c>
+      <c r="D60" t="n">
+        <v>192</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=fIEW47mq72EQ7kNvwGHmxOO&amp;_nc_oc=AdktyQYGcY_up_6ilyWId5PCyI7czi31jrI1F2-Mm1sOf5ZKtQkpUTclMfvTd-S8CkuyiUx-n4joQ11PNW0EA8Fs&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfKWulCIOiz0A_LAvM2BLagpc3bl0V92gV5F3nqIC4APlA&amp;oe=68457BAE</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2025-06-03 19:06:54.504787</t>
+        </is>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>45811</v>
+      </c>
+      <c r="I60" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K60" t="n">
+        <v>3</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>19:06:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>3075</v>
+      </c>
+      <c r="C61" t="n">
+        <v>246</v>
+      </c>
+      <c r="D61" t="n">
+        <v>193</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5uh9alQ2mvoQ7kNvwGsrUqv&amp;_nc_oc=AdnHPY9_wNQbE5LaT7Vwm1Sx57y28SXTUzYrc9Gt3yPXasPWnBnB4LFgfLBQHw6LftrwlrY0SOCK3eXS1Q907K75&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfPoaEXANGL025SK0GHAK6ppu99IHF6ITFNEkCPKGOPAdw&amp;oe=6846CD2E</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2025-06-04 19:07:14.580063</t>
+        </is>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>45812</v>
+      </c>
+      <c r="I61" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K61" t="n">
+        <v>4</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>19:07:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>3088</v>
+      </c>
+      <c r="C62" t="n">
+        <v>250</v>
+      </c>
+      <c r="D62" t="n">
+        <v>194</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5uh9alQ2mvoQ7kNvwFQI58I&amp;_nc_oc=AdnANzS_00TCWBZQoxfHlq1BKNFLOliRxvYdIHD06sYFm2Iy-kADPb4DPhk9dFI5JFkAgZQCCZTM1ut7drTBRHLV&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfNnlz4wkubAb_PMV2MOsSVnMFxFaWY_XokBQzqQ99JgWQ&amp;oe=68481EAE</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2025-06-05 19:07:34.819903</t>
+        </is>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>45813</v>
+      </c>
+      <c r="I62" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K62" t="n">
+        <v>5</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>19:07:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+✨ | ✧ 𝗹𝗼𝗰𝘀 ✧ (𝘀𝗲𝗹𝗳) 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>3127</v>
+      </c>
+      <c r="C63" t="n">
+        <v>250</v>
+      </c>
+      <c r="D63" t="n">
+        <v>195</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=5uh9alQ2mvoQ7kNvwFQI58I&amp;_nc_oc=AdnANzS_00TCWBZQoxfHlq1BKNFLOliRxvYdIHD06sYFm2Iy-kADPb4DPhk9dFI5JFkAgZQCCZTM1ut7drTBRHLV&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfOqnuVpOT-y5vMa17TgVNy7ZGoxW8bLkt7Ey-D9J2F7BQ&amp;oe=6849702E</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2025-06-06 19:06:57.568916</t>
+        </is>
+      </c>
+      <c r="H63" s="2" t="n">
+        <v>45814</v>
+      </c>
+      <c r="I63" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K63" t="n">
+        <v>6</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>19:06:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>3161</v>
+      </c>
+      <c r="C64" t="n">
+        <v>256</v>
+      </c>
+      <c r="D64" t="n">
+        <v>199</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>https://scontent-dfw5-2.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=0ceOn8XE-koQ7kNvwHcHIan&amp;_nc_oc=Adnk5jbmIo3ri_ox94hQVMLXUD8p-zLAhXcNU72cXe2d8xaR5NV-N_Q8mr9DeDNiCn2ELkYlc_CJCy-7wA0A5H-B&amp;_nc_zt=23&amp;_nc_ht=scontent-dfw5-2.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfPQOQZAF1QYsR2EszHWP7CysQ44aOnVcaN2gGGJJhYoAg&amp;oe=685120EE</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2025-06-12 17:53:23.378688</t>
+        </is>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>45820</v>
+      </c>
+      <c r="I64" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K64" t="n">
+        <v>12</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>17:53:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>3167</v>
+      </c>
+      <c r="C65" t="n">
+        <v>238</v>
+      </c>
+      <c r="D65" t="n">
+        <v>180</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=bT2qgR3wTE0Q7kNvwFfdDlw&amp;_nc_oc=AdkdyfllUTTK1XFqwomaw-9hUi862pQUOcdBlujeav0K52R7SvNQBpec5yjL8Uqo44EJuZV_gK0ZS9HmXbAhkYym&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfMmnvWGfwSTrAmCInk4plqLt78313yczkLyo_u7mgxY3g&amp;oe=6852726E</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2025-06-13 17:53:21.071878</t>
+        </is>
+      </c>
+      <c r="H65" s="2" t="n">
+        <v>45821</v>
+      </c>
+      <c r="I65" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K65" t="n">
+        <v>13</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>17:53:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>3178</v>
+      </c>
+      <c r="C66" t="n">
+        <v>238</v>
+      </c>
+      <c r="D66" t="n">
+        <v>180</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=bT2qgR3wTE0Q7kNvwH5fbBd&amp;_nc_oc=Adl6zM1K3OKJqcp0IpMPnQZtPnQbW1928lX8oGQWJFhHMaQhsPzlOsP7VsmCS5nRtPZ33k_JVmhjeOKgwd4mYxC8&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfNSonuk7cDkXaCP5AQ35mnWcJUt0kXS8v-xJ9HYn_2dpw&amp;oe=6853C3EE</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2025-06-14 17:52:56.712623</t>
+        </is>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>45822</v>
+      </c>
+      <c r="I66" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K66" t="n">
+        <v>14</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>17:52:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>3187</v>
+      </c>
+      <c r="C67" t="n">
+        <v>238</v>
+      </c>
+      <c r="D67" t="n">
+        <v>180</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=bT2qgR3wTE0Q7kNvwFMsRzx&amp;_nc_oc=Adk-sYAsA4-UnZEWJLxvufLISy83THEfAJSUmEnhmGDno9_7Vijn0QbU6hyTeu5DpgfPTYMkU4_NwyBgEGz4C81-&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfPKM0RV0AINDAixpVE3xRBA7K0fiUBR18lfwhqAqNakjA&amp;oe=6855156E</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2025-06-15 17:53:38.129469</t>
+        </is>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>45823</v>
+      </c>
+      <c r="I67" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K67" t="n">
+        <v>15</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>17:53:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>3188</v>
+      </c>
+      <c r="C68" t="n">
+        <v>236</v>
+      </c>
+      <c r="D68" t="n">
+        <v>180</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=QTwajCIG7CEQ7kNvwEUKjg0&amp;_nc_oc=AdlIl9EkcH-wuJfUesbTwzgAlPl5n0dHpKkLqXDrgoIvRo3cG4MU4fLNpF29e-rKNflYTdpzqdHd0volqcaAdxkH&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfOeSFshVALhv43rurjoF1u7WHaIj9VfaFKdT6rmrtW9Uw&amp;oe=685666EE</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2025-06-16 17:53:15.796292</t>
+        </is>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>45824</v>
+      </c>
+      <c r="I68" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K68" t="n">
+        <v>16</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>17:53:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>3190</v>
+      </c>
+      <c r="C69" t="n">
+        <v>236</v>
+      </c>
+      <c r="D69" t="n">
+        <v>181</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=QTwajCIG7CEQ7kNvwEUKjg0&amp;_nc_oc=AdlIl9EkcH-wuJfUesbTwzgAlPl5n0dHpKkLqXDrgoIvRo3cG4MU4fLNpF29e-rKNflYTdpzqdHd0volqcaAdxkH&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfOAnNLuXJSmEv-Bp3bLVT8i3u-24dOluCo_g2Lf9UtlaQ&amp;oe=6857B86E</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2025-06-17 17:53:33.886437</t>
+        </is>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>45825</v>
+      </c>
+      <c r="I69" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>17</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>17:53:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>3191</v>
+      </c>
+      <c r="C70" t="n">
+        <v>237</v>
+      </c>
+      <c r="D70" t="n">
+        <v>182</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=QTwajCIG7CEQ7kNvwHCHXko&amp;_nc_oc=AdnHhxHAgje0D962S4puFo4dQGgAdie3AsDy3GluX90CdHUSOaglKhwH0b7BQdPkLKXoozojMcXLA1r5GZBPrBYC&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfMTB3AN8B1ONTG3STT-pPuRwuWD2zrrkwYKSa0ZTu3Mag&amp;oe=685909EE</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2025-06-18 17:52:46.137621</t>
+        </is>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>45826</v>
+      </c>
+      <c r="I70" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K70" t="n">
+        <v>18</v>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>17:52:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>3207</v>
+      </c>
+      <c r="C71" t="n">
+        <v>238</v>
+      </c>
+      <c r="D71" t="n">
+        <v>182</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=7_HTIs3_9OgQ7kNvwGHtAf6&amp;_nc_oc=AdniuEPAtmrM9hICFvhkyOoNSW_PBPOVWDA4PaO4WrP5Vnoo3T5Vr1M3cSEO-soyoSA5Qmr-mhbVVlR3wheyczUk&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfNgGc-YFipDM0AyCZ6ZuSO6KEvkIjoGZoMnRrpkJVgDww&amp;oe=685A5B6E</t>
+        </is>
+      </c>
+      <c r="F71" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2025-06-19 17:53:30.579497</t>
+        </is>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>45827</v>
+      </c>
+      <c r="I71" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K71" t="n">
+        <v>19</v>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>17:53:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>3211</v>
+      </c>
+      <c r="C72" t="n">
+        <v>238</v>
+      </c>
+      <c r="D72" t="n">
+        <v>183</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=MA9s-L_wtdoQ7kNvwFd6YNO&amp;_nc_oc=Adlumd15we2nSwnVmTPzGtVuMz44FVX6i6wne5frY3YX4M_wqPfQh1NLZuv9p6u0UmZ_YzXDofUePCSnndhmI1Xv&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfPIeR6tFvmBTpuHbCU130_DXg7xhjH84by0QXgq6GVVMw&amp;oe=685FA16E</t>
+        </is>
+      </c>
+      <c r="F72" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>2025-06-23 18:38:50.764346</t>
+        </is>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>45831</v>
+      </c>
+      <c r="I72" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K72" t="n">
+        <v>23</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>18:38:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>3210</v>
+      </c>
+      <c r="C73" t="n">
+        <v>238</v>
+      </c>
+      <c r="D73" t="n">
+        <v>181</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=MA9s-L_wtdoQ7kNvwHPwaYQ&amp;_nc_oc=AdnvH0Rn91uV4RtNY84LTvfe3kP3ocjeh0YVeYIQammnnppSMl4vq02-7zJXZDDtHxcEtj1Ep-HFxJ4b1XJNcCdn&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfONwXNhd_u8nPYvzV5hbr65p2l8KqxVhlXB3nIq4EWdXA&amp;oe=6860F2EE</t>
+        </is>
+      </c>
+      <c r="F73" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>2025-06-24 18:39:10.600116</t>
+        </is>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>45832</v>
+      </c>
+      <c r="I73" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K73" t="n">
+        <v>24</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>18:39:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>3209</v>
+      </c>
+      <c r="C74" t="n">
+        <v>237</v>
+      </c>
+      <c r="D74" t="n">
+        <v>182</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tjBTf3eqEycQ7kNvwHTP-tE&amp;_nc_oc=AdkSygf6C4mhTySwVHnP3zV-TBP1SzLJSwI0J3GU4kKiRnJbnTd_g5l7ziE_CUfSYWxJdWVjtPGbWay--VcYKDpT&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfN0F1aaazSn0Pf8oKePJ-cT36erfO7YiscqMbg-7zMr0Q&amp;oe=6862446E</t>
+        </is>
+      </c>
+      <c r="F74" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>2025-06-25 18:38:42.838800</t>
+        </is>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>45833</v>
+      </c>
+      <c r="I74" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K74" t="n">
+        <v>25</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>18:38:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>3213</v>
+      </c>
+      <c r="C75" t="n">
+        <v>239</v>
+      </c>
+      <c r="D75" t="n">
+        <v>183</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tjBTf3eqEycQ7kNvwEsWPIC&amp;_nc_oc=Admy6x8bKiXNRD8G_UFFyQhORAI8hDzPCF_P8ZtKIcZ0XGPJdlLmE_oE3intWvZQ-1_JiqrGlKIlNmcGl3KqsnBH&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfN7owC2O8ThgOg7LoZ0XcVRM29WnytDvPhgtUqQsotvSw&amp;oe=686395EE</t>
+        </is>
+      </c>
+      <c r="F75" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>2025-06-26 18:51:30.617491</t>
+        </is>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>45834</v>
+      </c>
+      <c r="I75" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K75" t="n">
+        <v>26</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>18:51:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+💎 | ꜰᴏᴜɴᴅᴇʀ @themanepiece
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>3217</v>
+      </c>
+      <c r="C76" t="n">
+        <v>240</v>
+      </c>
+      <c r="D76" t="n">
+        <v>184</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=tjBTf3eqEycQ7kNvwG5mUMb&amp;_nc_oc=AdkRQdVPmDICfgoKWgsuR8FeCVfEIpVrAyriknsu4bdPzzMDUZyGmE45mnmZ6IbrBhf70rmBzw9FIwxteHnlUhi3&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfOR2qUbugEYRGE9PIJiyp9o4HbCiHoYpMAkM5E4i-PWmA&amp;oe=6864E76E</t>
+        </is>
+      </c>
+      <c r="F76" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>2025-06-27 18:39:20.997030</t>
+        </is>
+      </c>
+      <c r="H76" s="2" t="n">
+        <v>45835</v>
+      </c>
+      <c r="I76" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K76" t="n">
+        <v>27</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>18:39:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+💎 | @themanepiece
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>3213</v>
+      </c>
+      <c r="C77" t="n">
+        <v>240</v>
+      </c>
+      <c r="D77" t="n">
+        <v>184</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=HwA7iFTLzusQ7kNvwGsSeED&amp;_nc_oc=AdlP_zn7lWflDC1W2iREZcpR0Fv3USULxiyOH-spqb4KeOEQfAstxu-UQwyrrt3HWwzKAxng7LruJzVVzlzZ9QvX&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfMZ9PlDwAsw6CITc9ODuPilcjMZutb_1V78u59hmytPRg&amp;oe=686638EE</t>
+        </is>
+      </c>
+      <c r="F77" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>2025-06-28 18:39:17.803625</t>
+        </is>
+      </c>
+      <c r="H77" s="2" t="n">
+        <v>45836</v>
+      </c>
+      <c r="I77" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K77" t="n">
+        <v>28</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>18:39:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+💎 | @themanepiece
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>3209</v>
+      </c>
+      <c r="C78" t="n">
+        <v>240</v>
+      </c>
+      <c r="D78" t="n">
+        <v>185</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=HwA7iFTLzusQ7kNvwFcldEC&amp;_nc_oc=Adl3Gn9AHlswuL_-ngazfO9pMNOwdQl0IBSvy5D40NCowFBJkRx25VFHjUWUhjkyh0Vz2u_2jb_V3-AkY_FvJHYD&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfPdt2oPVjez86CDpsHB_mqJPlVydVsp9KJ49VcyZsd8gw&amp;oe=68678A6E</t>
+        </is>
+      </c>
+      <c r="F78" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>2025-06-29 18:39:08.329533</t>
+        </is>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>45837</v>
+      </c>
+      <c r="I78" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K78" t="n">
+        <v>29</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>18:39:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+💎 | @themanepiece
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>3214</v>
+      </c>
+      <c r="C79" t="n">
+        <v>242</v>
+      </c>
+      <c r="D79" t="n">
+        <v>185</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=HwA7iFTLzusQ7kNvwHbimjr&amp;_nc_oc=AdkstWkrV0tNWyN8SlY02-vJC4NDrx0IL6wj32Etatb00bF3-JWmqjX-ToJNoqX6zLwQkLsfMF08mi8FbXsqfMsf&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfNHRYdWVlzZ8BvDG8f80o7PoiEoUGGkT8N7XM1WxlYHTw&amp;oe=6868DBEE</t>
+        </is>
+      </c>
+      <c r="F79" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>2025-06-30 18:39:44.751295</t>
+        </is>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>45838</v>
+      </c>
+      <c r="I79" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="K79" t="n">
+        <v>30</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>18:39:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+💎 | @themanepiece
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>3216</v>
+      </c>
+      <c r="C80" t="n">
+        <v>242</v>
+      </c>
+      <c r="D80" t="n">
+        <v>186</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=EzyR6Zo_MpEQ7kNvwErF9XC&amp;_nc_oc=Adl4Z-IdNFbMS8KLEZ6Tjq2QECiAgKY6_DPIIqx0S9CJjJcDw02vQjVpCIcGmhhJ9-aEU4sE-1L7KuskePBX7p-b&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfPShl9QYowW1yD4AgsrLKHWD_FrBfKMmoMqI92xjfGVuA&amp;oe=686A2D6E</t>
+        </is>
+      </c>
+      <c r="F80" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>2025-07-01 18:39:32.233400</t>
+        </is>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>45839</v>
+      </c>
+      <c r="I80" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="K80" t="n">
+        <v>1</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>18:39:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+💎 | @themanepiece
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>3225</v>
+      </c>
+      <c r="C81" t="n">
+        <v>242</v>
+      </c>
+      <c r="D81" t="n">
+        <v>186</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=EzyR6Zo_MpEQ7kNvwFT8V-X&amp;_nc_oc=Adl2bepiO2xXIQLPgH1hMt57QAqKyuR-B5IbaALErItQvRkxye1E3Q6VSheUjObuobm67uUM7d78gLUJeYt08-x1&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfPibUBAsK8V3KYhKE8RGg7IDovqVd1QsYP1R4HTQHaqGw&amp;oe=686B7EEE</t>
+        </is>
+      </c>
+      <c r="F81" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>2025-07-02 18:40:56.535199</t>
+        </is>
+      </c>
+      <c r="H81" s="2" t="n">
+        <v>45840</v>
+      </c>
+      <c r="I81" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="K81" t="n">
+        <v>2</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>18:40:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>✧ 𝗹𝗼𝗰𝘀 ✧ 𝗹𝗶𝗯𝗲𝗿𝗮𝘁𝗶𝗼𝗻 ✧ 𝗹𝗶𝗳𝗲𝘀𝘁𝘆𝗹𝗲 ✧ 
+ʜᴇʟᴘɪɴɢ ʏᴏᴜ ᴍᴏᴠᴇ ғʀᴏᴍ ʜᴇsɪᴛᴀᴛɪᴏɴ ᴛᴏ ᴄʀᴇᴀᴛɪᴏɴ
+💎 | @themanepiece
+🪴 | 71 ʟᴏᴄs est. on 07.20.23
+📍 | ʜᴏᴜsᴛᴏɴ, ᴛx</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>3241</v>
+      </c>
+      <c r="C82" t="n">
+        <v>242</v>
+      </c>
+      <c r="D82" t="n">
+        <v>187</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>https://scontent-hou1-1.xx.fbcdn.net/v/t51.2885-15/481266977_997353345602937_1719041919639027270_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=7d201b&amp;_nc_ohc=jjjrhQ8TdewQ7kNvwF4y18N&amp;_nc_oc=Adltid0MJ3HRRo5dmViLIlKz7Qh6f46G2RiBlokHjyJCQNYZpiUdc30AZJK_pYKPXx4TMRsGj2Tm3KtYdxSc_udP&amp;_nc_zt=23&amp;_nc_ht=scontent-hou1-1.xx&amp;edm=AL-3X8kEAAAA&amp;oh=00_AfRH9abzcyx8savDlwqYzZy0IwdSkOi9q90HkO__HNNi_g&amp;oe=686F736E</t>
+        </is>
+      </c>
+      <c r="F82" t="n">
+        <v>1.784146145819126e+16</v>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>2025-07-05 17:39:23.842848</t>
+        </is>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>45843</v>
+      </c>
+      <c r="I82" t="n">
+        <v>2025</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="K82" t="n">
+        <v>5</v>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>17:39:23</t>
         </is>
       </c>
     </row>

</xml_diff>